<commit_message>
removed not so necessary folders and upated session with user food recommendation data
</commit_message>
<xml_diff>
--- a/data/user_log/food.xlsx
+++ b/data/user_log/food.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -708,7 +708,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45734.45154655602</v>
+        <v>45734.45154655092</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -807,6 +807,834 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>45734.5235596412</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Aarti</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>25</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>50</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Niacin, choline_total</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Vegetable
+  - Mushrooms, enoki, raw</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45734.52359769676</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Aarti</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>25</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>50</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G7" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Niacin, choline_total, vitamin_A</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Vegetable
+  - Mushrooms, enoki, raw</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>45734.52363763889</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Aarti</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>25</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>50</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G8" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Non-veg</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Niacin, choline_total, vitamin_A</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Turkey
+  - Turkey, whole, giblets, raw
+  - Turkey, gizzard, all classes, raw
+  - Turkey, drumstick, from whole bird, meat only, raw
+  - Turkey, retail parts, breast, meat and skin, raw
+  - Turkey, retail parts, breast, meat only, raw
+  - Turkey, whole, breast, meat only, raw
+  - Turkey, whole, light meat, meat and skin, raw
+  - Turkey, whole, meat only, raw
+  - Turkey, whole, meat and skin, raw
+  - Turkey from whole, light meat, meat and skin, with added solution, raw
+  - Turkey, whole, light meat, raw
+ Fish
+  - Fish, anchovy, european, raw
+  - Fish, tuna, fresh, yellowfin, raw
+  - Fish, tuna, fresh, bluefin, raw
+  - Fish, sturgeon, mixed species, raw
+  - Fish, shad, american, raw
+  - Fish, tuna, fresh, skipjack, raw
+  - Fish, mackerel, Pacific and jack, mixed species, raw
+ Lamb
+  - Veal, leg, top round, cap off, cutlet, boneless, raw
+  - Veal, leg (top round), separable lean and fat, raw
+  - Veal, sirloin, separable lean and fat, raw
+  - Veal, shoulder, arm, separable lean and fat, raw
+  - Lamb, ground, raw
+  - Veal, loin, separable lean only, raw
+  - Veal, shoulder, whole (arm and blade), separable lean and fat, raw
+  - Lamb, shoulder, whole (arm and blade), separable lean and fat, trimmed to 1/4" fat, choice, raw
+  - Veal, loin, separable lean and fat, raw
+  - Veal, shank, separable lean only, raw
+ Chicken
+  - Chicken, broilers or fryers, meat only, raw
+  - Chicken, broilers or fryers, meat and skin, raw
+  - Chicken, broilers or fryers, wing, meat only, raw
+  - Chicken, broilers or fryers, light meat, meat only, raw
+  - Chicken, broiler or fryers, breast, skinless, boneless, meat only, raw
+  - Chicken, roasting, giblets, raw
+  - Chicken, roasting, light meat, meat only, raw
+ Pork
+  - Pork, fresh, variety meats and by-products, stomach, raw
+ Vegetable
+  - Mushrooms, enoki, raw
+ Egg
+  - Egg, yolk, raw, fresh
+  - Egg, yolk, raw, frozen, sugared, pasteurized
+  - Egg, whole, raw, fresh</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45734.52923146991</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Aarti</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>25</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>50</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G9" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>cholesterol, folate_total</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Vegetable
+  - Arrowroot, raw
+  - Asparagus, green, raw
+  - Chrysanthemum leaves, raw
+  - Epazote, raw
+  - Cowpeas (blackeyes), immature seeds, raw
+  - Mustard spinach, (tendergreen), raw
+  - Seaweed, kelp, raw
+  - Arugula, baby, raw
+  - Seaweed, wakame, raw
+  - Lettuce, cos or romaine, raw
+  - Seaweed, laver, raw
+  - Endive, raw
+  - Beans, fava, in pod, raw
+  - Vinespinach, (basella), raw
+  - Chrysanthemum, garland, raw
+  - Soybeans, mature seeds, sprouted, raw
+  - Beets, raw
+  - Turnip greens, raw
+ Legumes
+  - Chickpeas (garbanzo beans, bengal gram), mature seeds, raw
+  - Beans, adzuki, mature seeds, raw
+  - Mung beans, mature seeds, raw
+  - Beans, kidney, royal red, mature seeds, raw
+  - Beans, cranberry (roman), mature seeds, raw
+  - Beans, french, mature seeds, raw
+ Fruit
+  - Avocado, Hass, peeled, raw
+ Grain
+  - Rice, white, long-grain, regular, raw, enriched</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45734.5320956713</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Aarti</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>25</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>50</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G10" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>cholesterol, folate_total</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Vegetable
+  - Arrowroot, raw
+  - Asparagus, green, raw
+  - Chrysanthemum leaves, raw
+  - Epazote, raw
+  - Cowpeas (blackeyes), immature seeds, raw
+  - Mustard spinach, (tendergreen), raw
+  - Seaweed, kelp, raw
+  - Arugula, baby, raw
+  - Seaweed, wakame, raw
+  - Lettuce, cos or romaine, raw
+  - Seaweed, laver, raw
+  - Endive, raw
+  - Beans, fava, in pod, raw
+  - Vinespinach, (basella), raw
+  - Chrysanthemum, garland, raw
+  - Soybeans, mature seeds, sprouted, raw
+  - Beets, raw
+  - Turnip greens, raw
+ Legumes
+  - Chickpeas (garbanzo beans, bengal gram), mature seeds, raw
+  - Beans, adzuki, mature seeds, raw
+  - Mung beans, mature seeds, raw
+  - Beans, kidney, royal red, mature seeds, raw
+  - Beans, cranberry (roman), mature seeds, raw
+  - Beans, french, mature seeds, raw
+ Fruit
+  - Avocado, Hass, peeled, raw
+ Grain
+  - Rice, white, long-grain, regular, raw, enriched</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45734.53968447917</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Aarti</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>25</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>50</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G11" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>riboflavin, cholesterol, folate_total</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Legumes
+  - Chickpeas (garbanzo beans, bengal gram), mature seeds, raw
+  - Beans, adzuki, mature seeds, raw
+  - Mung beans, mature seeds, raw
+  - Beans, kidney, royal red, mature seeds, raw
+  - Beans, cranberry (roman), mature seeds, raw
+ Vegetable
+  - Arrowroot, raw
+  - Epazote, raw
+  - Seaweed, laver, raw
+  - Seaweed, irishmoss, raw
+  - Chrysanthemum leaves, raw
+  - Beans, fava, in pod, raw
+  - Seaweed, wakame, raw
+  - Cowpeas (blackeyes), immature seeds, raw
+  - Taro leaves, raw
+  - Asparagus, green, raw
+  - Seaweed, kelp, raw
+  - Mustard spinach, (tendergreen), raw
+ Fruit
+  - Grapes, muscadine, raw
+ Cheese
+  - Cheese, brie</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45734.54106072916</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Ary</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>25</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>50</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G12" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>copper, vitamin_E</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Vegetable
+  - Peppers, jalapeno, raw
+  - Radicchio, raw
+  - Taro, raw
+  - Turnip greens, raw
+  - Coriander (cilantro) leaves, raw
+  - Chicory greens, raw
+  - Mustard greens, raw
+  - Taro leaves, raw
+  - Parsnips, raw
+  - Peppers, sweet, red, raw
+  - Squash, winter, butternut, raw
+  - Grape leaves, raw
+  - Asparagus, raw
+  - Broccoli raab, raw
+  - Waterchestnuts, chinese, (matai), raw
+  - Pumpkin, raw
+  - Collards, raw
+ Fruit
+  - Avocados, raw, Florida
+  - Avocados, raw, all commercial varieties
+  - Avocados, raw, California
+  - Kiwifruit, green, raw
+  - Kiwifruit, ZESPRI SunGold, raw
+  - Kiwifruit, green, raw
+  - Cranberries, raw
+  - Blackberries, raw
+  - Sapote, mamey, raw
+ Butter
+  - Butter, without salt
+  - Butter, salted
+  - Butter, whipped, with salt
+ Cream
+  - Cream substitute, flavored, liquid
+ Legumes
+  - Peanuts, all types, raw
+ Dressing
+  - Sour dressing, non-butterfat, cultured, filled cream-type</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>45734.54313627315</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>aarti</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>25</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>50</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G13" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>selenium, vitamin_D</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Vegetable
+  - Mushrooms, brown, italian, or crimini, exposed to ultraviolet light, raw
+  - Mushrooms, portabella, exposed to ultraviolet light, raw
+  - Mushroom, white, exposed to ultraviolet light, raw
+  - Mushrooms, maitake, raw
+  - Mushrooms, Chanterelle, raw</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>45734.54339240741</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>arha</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>25</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>50</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G14" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>selenium</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Nuts
+  - Nuts, macadamia nuts, raw</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>45734.54511746528</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Aarti</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>25</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>50</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G15" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>vitamin_B_6, choline_total, vitamin_A</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Vegetable
+  - Garlic, raw
+  - Drumstick leaves, raw
+  - Balsam-pear (bitter gourd), leafy tips, raw
+  - Hearts of palm, raw
+ Fruit
+  - Sapote, mamey, raw</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>45734.54562295139</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Aarti</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>25</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>50</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G16" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>vitamin_D</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Vegetable
+  - Mushrooms, portabella, exposed to ultraviolet light, raw
+  - Mushrooms, brown, italian, or crimini, exposed to ultraviolet light, raw
+  - Mushroom, white, exposed to ultraviolet light, raw
+  - Mushrooms, maitake, raw
+  - Mushrooms, Chanterelle, raw
+  - Mushrooms, morel, raw
+ Milk
+  - Milk, evaporated, 2% fat, with added vitamin A and vitamin D
+  - Milk, low sodium, fluid
+  - Milk, whole, 3.25% milkfat, with added vitamin D
+ Cream
+  - Cream, fluid, heavy whipping</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>45734.54574659722</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Aarti</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>25</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>50</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G17" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>vitamin_D</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Vegetable
+  - Mushrooms, portabella, exposed to ultraviolet light, raw
+  - Mushrooms, brown, italian, or crimini, exposed to ultraviolet light, raw
+  - Mushroom, white, exposed to ultraviolet light, raw
+  - Mushrooms, maitake, raw
+  - Mushrooms, Chanterelle, raw
+  - Mushrooms, morel, raw
+ Milk
+  - Milk, evaporated, 2% fat, with added vitamin A and vitamin D
+  - Milk, low sodium, fluid
+  - Milk, whole, 3.25% milkfat, with added vitamin D
+ Cream
+  - Cream, fluid, heavy whipping</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>45734.54633281802</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Aarti</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>25</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>50</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="G18" t="n">
+        <v>22.22</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Normal weight - Maintain a balanced diet and exercise.</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>riboflavin, Niacin</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+ Fruit
+  - Grapes, muscadine, raw
+ Vegetable
+  - Mushrooms, enoki, raw</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>